<commit_message>
included files jul 30, 2022
</commit_message>
<xml_diff>
--- a/painelcnj/indicadores/Cno-2g.xlsx
+++ b/painelcnj/indicadores/Cno-2g.xlsx
@@ -371,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,102 +402,170 @@
     <row r="2" ht="13.073974609375" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>97.898</t>
+          <t>21.938</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>97.898</t>
+          <t>21.938</t>
         </is>
       </c>
     </row>
     <row r="3" ht="13.073974609375" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>1.013.960</t>
+          <t>63.615</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>1.013.960</t>
+          <t>63.615</t>
         </is>
       </c>
     </row>
     <row r="4" ht="13.073974609375" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>146.612</t>
+          <t>22.169</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>146.612</t>
+          <t>22.169</t>
         </is>
       </c>
     </row>
     <row r="5" ht="13.073974609375" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>197.367</t>
+          <t>58.877</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>197.367</t>
+          <t>58.877</t>
         </is>
       </c>
     </row>
     <row r="6" ht="13.073974609375" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>63.765</t>
+          <t>11.804</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>63.765</t>
+          <t>11.804</t>
         </is>
       </c>
     </row>
     <row r="7" ht="13.073974609375" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>46.031</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>46.031</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="13.073974609375" customHeight="1">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>27.422</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>27.422</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="13.073974609375" customHeight="1">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>73.156</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>73.156</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="13.073974609375" customHeight="1">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>6.968</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>6.968</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="13.073974609375" customHeight="1">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
           <t>2020</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>1.335.013</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>1.335.013</t>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>42.495</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>42.495</t>
         </is>
       </c>
     </row>

</xml_diff>